<commit_message>
data collection for 11-14 basically done, some incorrect QB data that I have to correct but otherwise good
</commit_message>
<xml_diff>
--- a/star players notes.xlsx
+++ b/star players notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="318">
   <si>
     <t>Team</t>
   </si>
@@ -256,6 +256,720 @@
   </si>
   <si>
     <t>Painter started 3-11, orlovsky 12-16, Collins 1-3</t>
+  </si>
+  <si>
+    <t>Pierre Garcon</t>
+  </si>
+  <si>
+    <t>Donald Brown</t>
+  </si>
+  <si>
+    <t>Reggie Wayne</t>
+  </si>
+  <si>
+    <t>Vick Ballard</t>
+  </si>
+  <si>
+    <t>T.Y. Hilton</t>
+  </si>
+  <si>
+    <t>Coby Fleener</t>
+  </si>
+  <si>
+    <t>Dwayne Allen</t>
+  </si>
+  <si>
+    <t>Ahmad Bradshaw</t>
+  </si>
+  <si>
+    <t>OTI</t>
+  </si>
+  <si>
+    <t>Nate Washington</t>
+  </si>
+  <si>
+    <t>Damian Williams</t>
+  </si>
+  <si>
+    <t>Chris Johnson</t>
+  </si>
+  <si>
+    <t>this is where I started getting the right qb data</t>
+  </si>
+  <si>
+    <t>Kendall Wright</t>
+  </si>
+  <si>
+    <t>Hasselbeck</t>
+  </si>
+  <si>
+    <t>QB</t>
+  </si>
+  <si>
+    <t>Fitzpatrick, Locker</t>
+  </si>
+  <si>
+    <t>Delanie Walker</t>
+  </si>
+  <si>
+    <t>Justin Hunter</t>
+  </si>
+  <si>
+    <t>WhiteHurst, Mettenberger, Locker</t>
+  </si>
+  <si>
+    <t>JAX</t>
+  </si>
+  <si>
+    <t>Gabbert, McCown</t>
+  </si>
+  <si>
+    <t>Maurice Jones-Drew</t>
+  </si>
+  <si>
+    <t>Jason Hill</t>
+  </si>
+  <si>
+    <t>Chastin West</t>
+  </si>
+  <si>
+    <t>Henne, Gabbert</t>
+  </si>
+  <si>
+    <t>Cecil Shorts</t>
+  </si>
+  <si>
+    <t>Justin Blackmon</t>
+  </si>
+  <si>
+    <t>Marcedes Lewis</t>
+  </si>
+  <si>
+    <t>Henne, Bortles</t>
+  </si>
+  <si>
+    <t>Allen Hurns</t>
+  </si>
+  <si>
+    <t>Denard Robinson</t>
+  </si>
+  <si>
+    <t>Allen Robinson</t>
+  </si>
+  <si>
+    <t>HTX</t>
+  </si>
+  <si>
+    <t>Schaub, Yates, Leinart</t>
+  </si>
+  <si>
+    <t>Arian Foster</t>
+  </si>
+  <si>
+    <t>Owen Daniels</t>
+  </si>
+  <si>
+    <t>Schaub</t>
+  </si>
+  <si>
+    <t>Andre Johnson</t>
+  </si>
+  <si>
+    <t>Schaub, Keenum</t>
+  </si>
+  <si>
+    <t>Garrett Graham</t>
+  </si>
+  <si>
+    <t>Fitzpatrick, Keenum, Mallett</t>
+  </si>
+  <si>
+    <t>DeAndre Hopkins</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>Tebow, Orton</t>
+  </si>
+  <si>
+    <t>Willis MaGahee</t>
+  </si>
+  <si>
+    <t>Demaryius Thomas</t>
+  </si>
+  <si>
+    <t>Manning</t>
+  </si>
+  <si>
+    <t>Brandon Stokely</t>
+  </si>
+  <si>
+    <t>Knowshon Moreno</t>
+  </si>
+  <si>
+    <t>Julius Thomas</t>
+  </si>
+  <si>
+    <t>C.J. Anderson</t>
+  </si>
+  <si>
+    <t>RAI</t>
+  </si>
+  <si>
+    <t>Palmer, Campbell, Boller</t>
+  </si>
+  <si>
+    <t>Michael Bush</t>
+  </si>
+  <si>
+    <t>Denarius Moore</t>
+  </si>
+  <si>
+    <t>Darren McFadden</t>
+  </si>
+  <si>
+    <t>Brandon Myers</t>
+  </si>
+  <si>
+    <t>Palmer, Pryor</t>
+  </si>
+  <si>
+    <t>Pryor, McGloin, Flynn</t>
+  </si>
+  <si>
+    <t>Rashad Jennings</t>
+  </si>
+  <si>
+    <t>Carr</t>
+  </si>
+  <si>
+    <t>James Jones</t>
+  </si>
+  <si>
+    <t>Andre Holmes</t>
+  </si>
+  <si>
+    <t>Mychal Rivera</t>
+  </si>
+  <si>
+    <t>KAN</t>
+  </si>
+  <si>
+    <t>Cassel, Palko, Orton (note overlap with DEN)</t>
+  </si>
+  <si>
+    <t>Dwayne Bowe</t>
+  </si>
+  <si>
+    <t>Jackie Battle</t>
+  </si>
+  <si>
+    <t>Steve Breaston</t>
+  </si>
+  <si>
+    <t>Cassel, Quinn</t>
+  </si>
+  <si>
+    <t>Jamaal Charles</t>
+  </si>
+  <si>
+    <t>Shaun Draughn</t>
+  </si>
+  <si>
+    <t>Smith, Daniel in game 16</t>
+  </si>
+  <si>
+    <t>Knile Davis</t>
+  </si>
+  <si>
+    <t>Travis Kelce</t>
+  </si>
+  <si>
+    <t>SDG</t>
+  </si>
+  <si>
+    <t>Rivers</t>
+  </si>
+  <si>
+    <t>Mike Tolbert</t>
+  </si>
+  <si>
+    <t>Vincent Jackson</t>
+  </si>
+  <si>
+    <t>Antonio Gates</t>
+  </si>
+  <si>
+    <t>Danario Alexander</t>
+  </si>
+  <si>
+    <t>Malcom Floyd</t>
+  </si>
+  <si>
+    <t>Keenan Allen</t>
+  </si>
+  <si>
+    <t>Eddie Royal</t>
+  </si>
+  <si>
+    <t>Danny Woodhead</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>Laurent Robinson</t>
+  </si>
+  <si>
+    <t>Dez Bryant</t>
+  </si>
+  <si>
+    <t>Miles Austin</t>
+  </si>
+  <si>
+    <t>Romo</t>
+  </si>
+  <si>
+    <t>Felix Jones</t>
+  </si>
+  <si>
+    <t>Jason Witten</t>
+  </si>
+  <si>
+    <t>DeMarco Murray</t>
+  </si>
+  <si>
+    <t>Romo with Weeden in one</t>
+  </si>
+  <si>
+    <t>Terrence Williams</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
+    <t>Vick and Young</t>
+  </si>
+  <si>
+    <t>LeSean McCoy</t>
+  </si>
+  <si>
+    <t>Jeremy Maclin</t>
+  </si>
+  <si>
+    <t>Brent Celek</t>
+  </si>
+  <si>
+    <t>Vick, Foles</t>
+  </si>
+  <si>
+    <t>Bryce Brown</t>
+  </si>
+  <si>
+    <t>Foles, Vick</t>
+  </si>
+  <si>
+    <t>DeSean Jackson</t>
+  </si>
+  <si>
+    <t>Riley Cooper</t>
+  </si>
+  <si>
+    <t>Foles, Sanchez</t>
+  </si>
+  <si>
+    <t>Jordan Matthews</t>
+  </si>
+  <si>
+    <t>Darren Sproles</t>
+  </si>
+  <si>
+    <t>NYG</t>
+  </si>
+  <si>
+    <t>Victor Cruz</t>
+  </si>
+  <si>
+    <t>Brandon Jacobs</t>
+  </si>
+  <si>
+    <t>Andre Brown</t>
+  </si>
+  <si>
+    <t>Rueben Randle</t>
+  </si>
+  <si>
+    <t>Odell Beckham</t>
+  </si>
+  <si>
+    <t>Andre Williams</t>
+  </si>
+  <si>
+    <t>Larry Donnell</t>
+  </si>
+  <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>Jabar Gaffney</t>
+  </si>
+  <si>
+    <t>Santana Moss</t>
+  </si>
+  <si>
+    <t>Roy Helu</t>
+  </si>
+  <si>
+    <t>Grossman, Beck</t>
+  </si>
+  <si>
+    <t>RG3, Cousins</t>
+  </si>
+  <si>
+    <t>Alfred Morris</t>
+  </si>
+  <si>
+    <t>RG3, Cousins, McCoy</t>
+  </si>
+  <si>
+    <t>GNB</t>
+  </si>
+  <si>
+    <t>Rodgers, Flynn in one</t>
+  </si>
+  <si>
+    <t>Jordy Nelson</t>
+  </si>
+  <si>
+    <t>Greg Jennings</t>
+  </si>
+  <si>
+    <t>Jermichael Finley</t>
+  </si>
+  <si>
+    <t>Rodgers</t>
+  </si>
+  <si>
+    <t>Eddie Lacy</t>
+  </si>
+  <si>
+    <t>Randall Cobb</t>
+  </si>
+  <si>
+    <t>Rodgers, Flynn, Tolzien, Wallace</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>Adrian Peterson</t>
+  </si>
+  <si>
+    <t>Percy Harvin</t>
+  </si>
+  <si>
+    <t>Toby Gerhart</t>
+  </si>
+  <si>
+    <t>Ponder, McNabb</t>
+  </si>
+  <si>
+    <t>Ponder</t>
+  </si>
+  <si>
+    <t>Kyle Rudolph</t>
+  </si>
+  <si>
+    <t>Ponder, Cassel, Freeman</t>
+  </si>
+  <si>
+    <t>Cordarrelle Patterson</t>
+  </si>
+  <si>
+    <t>Bridgewater, Cassel, Ponder</t>
+  </si>
+  <si>
+    <t>Matt Asiata</t>
+  </si>
+  <si>
+    <t>Jarius Wright</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>Cutler, Hanie, McCown</t>
+  </si>
+  <si>
+    <t>Marion Barber</t>
+  </si>
+  <si>
+    <t>Kellen Davis</t>
+  </si>
+  <si>
+    <t>Matt Forte</t>
+  </si>
+  <si>
+    <t>Cutler, Campbell</t>
+  </si>
+  <si>
+    <t>Cutler, McCown</t>
+  </si>
+  <si>
+    <t>Alshon Jeffery</t>
+  </si>
+  <si>
+    <t>Cutler, Classen</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>Stafford</t>
+  </si>
+  <si>
+    <t>Calvin Johnson</t>
+  </si>
+  <si>
+    <t>Kevin Smith</t>
+  </si>
+  <si>
+    <t>Titus Young</t>
+  </si>
+  <si>
+    <t>Mikel Leshoure</t>
+  </si>
+  <si>
+    <t>Brandon Pettigrew</t>
+  </si>
+  <si>
+    <t>Joique Bell</t>
+  </si>
+  <si>
+    <t>Golden Tate</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>Newton</t>
+  </si>
+  <si>
+    <t>DeAngelo Williams</t>
+  </si>
+  <si>
+    <t>Jonathan Stewart</t>
+  </si>
+  <si>
+    <t>Greg Olsen</t>
+  </si>
+  <si>
+    <t>Newton, Anderson</t>
+  </si>
+  <si>
+    <t>Kelvin Benjamin</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Michael Turner</t>
+  </si>
+  <si>
+    <t>Roddy White</t>
+  </si>
+  <si>
+    <t>Julio Jones</t>
+  </si>
+  <si>
+    <t>Tony Gonzalez</t>
+  </si>
+  <si>
+    <t>Steven Jackson</t>
+  </si>
+  <si>
+    <t>Jacquizz Rodgers</t>
+  </si>
+  <si>
+    <t>TAM</t>
+  </si>
+  <si>
+    <t>Freeman, Johnson</t>
+  </si>
+  <si>
+    <t>Dezmon Briscoe</t>
+  </si>
+  <si>
+    <t>LaGarrette Blount</t>
+  </si>
+  <si>
+    <t>Freeman</t>
+  </si>
+  <si>
+    <t>Doug Martin</t>
+  </si>
+  <si>
+    <t>Mike Williams</t>
+  </si>
+  <si>
+    <t>Bobby Rainey</t>
+  </si>
+  <si>
+    <t>Tim Rainey</t>
+  </si>
+  <si>
+    <t>Glennon, Freeman</t>
+  </si>
+  <si>
+    <t>McCown, Glennon</t>
+  </si>
+  <si>
+    <t>Mike Evans</t>
+  </si>
+  <si>
+    <t>NOR</t>
+  </si>
+  <si>
+    <t>Jimmy Graham</t>
+  </si>
+  <si>
+    <t>Marques Colston</t>
+  </si>
+  <si>
+    <t>Brees</t>
+  </si>
+  <si>
+    <t>Daren Sproles</t>
+  </si>
+  <si>
+    <t>Pierre Thomas</t>
+  </si>
+  <si>
+    <t>Mark Ingram</t>
+  </si>
+  <si>
+    <t>CRD</t>
+  </si>
+  <si>
+    <t>Skelton, Kolb</t>
+  </si>
+  <si>
+    <t>Beanie Wells</t>
+  </si>
+  <si>
+    <t>Larry Fitzgerald</t>
+  </si>
+  <si>
+    <t>Early Doucet</t>
+  </si>
+  <si>
+    <t>Skelton, Kolb, Lindley, Hoyer</t>
+  </si>
+  <si>
+    <t>Andre Roberts</t>
+  </si>
+  <si>
+    <t>Palmer</t>
+  </si>
+  <si>
+    <t>Michael Floyd</t>
+  </si>
+  <si>
+    <t>Stanton, Palmer, Lindley</t>
+  </si>
+  <si>
+    <t>Andre Ellington</t>
+  </si>
+  <si>
+    <t>John Brown</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>Bradford, Feeley, Clemens</t>
+  </si>
+  <si>
+    <t>Bradford</t>
+  </si>
+  <si>
+    <t>Brandon Lloyd</t>
+  </si>
+  <si>
+    <t>Brandon Gibson</t>
+  </si>
+  <si>
+    <t>Lance Kendricks</t>
+  </si>
+  <si>
+    <t>Bradford, Clemens</t>
+  </si>
+  <si>
+    <t>Zac Stacy</t>
+  </si>
+  <si>
+    <t>Jared Cook</t>
+  </si>
+  <si>
+    <t>Tavon Austin</t>
+  </si>
+  <si>
+    <t>Davis, Hill</t>
+  </si>
+  <si>
+    <t>Tre Mason</t>
+  </si>
+  <si>
+    <t>Benny Cunningham</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>Jackson, Whitehurst</t>
+  </si>
+  <si>
+    <t>Marshawn Lynch</t>
+  </si>
+  <si>
+    <t>Doug Baldwin</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Sidney Rice</t>
+  </si>
+  <si>
+    <t>Luke Wilson</t>
+  </si>
+  <si>
+    <t>SFO</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Vernon Davis</t>
+  </si>
+  <si>
+    <t>Frank Gore</t>
+  </si>
+  <si>
+    <t>Michael Crabtree</t>
+  </si>
+  <si>
+    <t>Smith, Kaepernick</t>
+  </si>
+  <si>
+    <t>Anquan Boldin</t>
+  </si>
+  <si>
+    <t>Kaepernick</t>
   </si>
 </sst>
 </file>
@@ -594,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:L160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,9 +1320,10 @@
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,8 +1339,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -642,7 +1360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -659,7 +1377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -676,7 +1394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -693,7 +1411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -710,7 +1428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -727,7 +1445,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -744,7 +1462,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -761,7 +1479,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -778,7 +1496,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -795,7 +1513,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -812,7 +1530,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1053,7 +1771,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -1073,7 +1791,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1093,7 +1811,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -1113,7 +1831,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1130,7 +1848,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1147,7 +1865,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1164,7 +1882,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -1181,39 +1899,1861 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>78</v>
       </c>
       <c r="B42">
         <v>2011</v>
       </c>
+      <c r="C42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" t="s">
+        <v>82</v>
+      </c>
       <c r="F42" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>78</v>
       </c>
       <c r="B43">
         <v>2012</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>78</v>
       </c>
       <c r="B44">
         <v>2013</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>78</v>
       </c>
       <c r="B45">
         <v>2014</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47">
+        <v>2011</v>
+      </c>
+      <c r="C47" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" t="s">
+        <v>91</v>
+      </c>
+      <c r="F47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48">
+        <v>2012</v>
+      </c>
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" t="s">
+        <v>93</v>
+      </c>
+      <c r="F48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49">
+        <v>2013</v>
+      </c>
+      <c r="C49" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" t="s">
+        <v>97</v>
+      </c>
+      <c r="E49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50">
+        <v>2014</v>
+      </c>
+      <c r="C50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" t="s">
+        <v>98</v>
+      </c>
+      <c r="F50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52">
+        <v>2011</v>
+      </c>
+      <c r="C52" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" t="s">
+        <v>104</v>
+      </c>
+      <c r="F52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53">
+        <v>2012</v>
+      </c>
+      <c r="C53" t="s">
+        <v>106</v>
+      </c>
+      <c r="D53" t="s">
+        <v>107</v>
+      </c>
+      <c r="E53" t="s">
+        <v>108</v>
+      </c>
+      <c r="F53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54">
+        <v>2013</v>
+      </c>
+      <c r="C54" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" t="s">
+        <v>108</v>
+      </c>
+      <c r="E54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55">
+        <v>2014</v>
+      </c>
+      <c r="C55" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" t="s">
+        <v>111</v>
+      </c>
+      <c r="E55" t="s">
+        <v>112</v>
+      </c>
+      <c r="F55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57">
+        <v>2011</v>
+      </c>
+      <c r="C57" t="s">
+        <v>115</v>
+      </c>
+      <c r="D57" t="s">
+        <v>69</v>
+      </c>
+      <c r="E57" t="s">
+        <v>116</v>
+      </c>
+      <c r="F57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58">
+        <v>2012</v>
+      </c>
+      <c r="C58" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" t="s">
+        <v>116</v>
+      </c>
+      <c r="E58" t="s">
+        <v>118</v>
+      </c>
+      <c r="F58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59">
+        <v>2013</v>
+      </c>
+      <c r="C59" t="s">
+        <v>118</v>
+      </c>
+      <c r="D59" t="s">
+        <v>120</v>
+      </c>
+      <c r="E59" t="s">
+        <v>69</v>
+      </c>
+      <c r="F59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60">
+        <v>2014</v>
+      </c>
+      <c r="C60" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" t="s">
+        <v>122</v>
+      </c>
+      <c r="E60" t="s">
+        <v>118</v>
+      </c>
+      <c r="F60" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62">
+        <v>2011</v>
+      </c>
+      <c r="C62" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" t="s">
+        <v>125</v>
+      </c>
+      <c r="E62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63">
+        <v>2012</v>
+      </c>
+      <c r="C63" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" t="s">
+        <v>126</v>
+      </c>
+      <c r="E63" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64">
+        <v>2013</v>
+      </c>
+      <c r="C64" t="s">
+        <v>126</v>
+      </c>
+      <c r="D64" t="s">
+        <v>129</v>
+      </c>
+      <c r="E64" t="s">
+        <v>130</v>
+      </c>
+      <c r="F64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>123</v>
+      </c>
+      <c r="B65">
+        <v>2014</v>
+      </c>
+      <c r="C65" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65" t="s">
+        <v>126</v>
+      </c>
+      <c r="E65" t="s">
+        <v>131</v>
+      </c>
+      <c r="F65" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67">
+        <v>2011</v>
+      </c>
+      <c r="C67" t="s">
+        <v>134</v>
+      </c>
+      <c r="D67" t="s">
+        <v>135</v>
+      </c>
+      <c r="E67" t="s">
+        <v>136</v>
+      </c>
+      <c r="F67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68">
+        <v>2012</v>
+      </c>
+      <c r="C68" t="s">
+        <v>135</v>
+      </c>
+      <c r="D68" t="s">
+        <v>137</v>
+      </c>
+      <c r="E68" t="s">
+        <v>136</v>
+      </c>
+      <c r="F68" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69">
+        <v>2013</v>
+      </c>
+      <c r="C69" t="s">
+        <v>140</v>
+      </c>
+      <c r="D69" t="s">
+        <v>135</v>
+      </c>
+      <c r="E69" t="s">
+        <v>136</v>
+      </c>
+      <c r="F69" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>132</v>
+      </c>
+      <c r="B70">
+        <v>2014</v>
+      </c>
+      <c r="C70" t="s">
+        <v>142</v>
+      </c>
+      <c r="D70" t="s">
+        <v>143</v>
+      </c>
+      <c r="E70" t="s">
+        <v>144</v>
+      </c>
+      <c r="F70" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72">
+        <v>2011</v>
+      </c>
+      <c r="C72" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" t="s">
+        <v>149</v>
+      </c>
+      <c r="E72" t="s">
+        <v>148</v>
+      </c>
+      <c r="F72" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73">
+        <v>2012</v>
+      </c>
+      <c r="C73" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73" t="s">
+        <v>147</v>
+      </c>
+      <c r="E73" t="s">
+        <v>152</v>
+      </c>
+      <c r="F73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74">
+        <v>2013</v>
+      </c>
+      <c r="C74" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74" t="s">
+        <v>147</v>
+      </c>
+      <c r="E74" t="s">
+        <v>154</v>
+      </c>
+      <c r="F74" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75">
+        <v>2014</v>
+      </c>
+      <c r="C75" t="s">
+        <v>151</v>
+      </c>
+      <c r="D75" t="s">
+        <v>154</v>
+      </c>
+      <c r="E75" t="s">
+        <v>155</v>
+      </c>
+      <c r="F75" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>156</v>
+      </c>
+      <c r="B77">
+        <v>2011</v>
+      </c>
+      <c r="C77" t="s">
+        <v>158</v>
+      </c>
+      <c r="D77" t="s">
+        <v>159</v>
+      </c>
+      <c r="E77" t="s">
+        <v>160</v>
+      </c>
+      <c r="F77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>156</v>
+      </c>
+      <c r="B78">
+        <v>2012</v>
+      </c>
+      <c r="C78" t="s">
+        <v>160</v>
+      </c>
+      <c r="D78" t="s">
+        <v>161</v>
+      </c>
+      <c r="E78" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79">
+        <v>2013</v>
+      </c>
+      <c r="C79" t="s">
+        <v>163</v>
+      </c>
+      <c r="D79" t="s">
+        <v>164</v>
+      </c>
+      <c r="E79" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80">
+        <v>2014</v>
+      </c>
+      <c r="C80" t="s">
+        <v>160</v>
+      </c>
+      <c r="D80" t="s">
+        <v>164</v>
+      </c>
+      <c r="E80" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>166</v>
+      </c>
+      <c r="B82">
+        <v>2011</v>
+      </c>
+      <c r="C82" t="s">
+        <v>167</v>
+      </c>
+      <c r="D82" t="s">
+        <v>168</v>
+      </c>
+      <c r="E82" t="s">
+        <v>169</v>
+      </c>
+      <c r="F82" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>166</v>
+      </c>
+      <c r="B83">
+        <v>2012</v>
+      </c>
+      <c r="C83" t="s">
+        <v>168</v>
+      </c>
+      <c r="D83" t="s">
+        <v>169</v>
+      </c>
+      <c r="E83" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84">
+        <v>2013</v>
+      </c>
+      <c r="C84" t="s">
+        <v>168</v>
+      </c>
+      <c r="D84" t="s">
+        <v>173</v>
+      </c>
+      <c r="E84" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>166</v>
+      </c>
+      <c r="B85">
+        <v>2014</v>
+      </c>
+      <c r="C85" t="s">
+        <v>168</v>
+      </c>
+      <c r="D85" t="s">
+        <v>173</v>
+      </c>
+      <c r="E85" t="s">
+        <v>175</v>
+      </c>
+      <c r="F85" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>176</v>
+      </c>
+      <c r="B87">
+        <v>2011</v>
+      </c>
+      <c r="C87" t="s">
+        <v>178</v>
+      </c>
+      <c r="D87" t="s">
+        <v>179</v>
+      </c>
+      <c r="E87" t="s">
+        <v>180</v>
+      </c>
+      <c r="F87" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88">
+        <v>2012</v>
+      </c>
+      <c r="C88" t="s">
+        <v>179</v>
+      </c>
+      <c r="D88" t="s">
+        <v>178</v>
+      </c>
+      <c r="E88" t="s">
+        <v>182</v>
+      </c>
+      <c r="F88" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89">
+        <v>2013</v>
+      </c>
+      <c r="C89" t="s">
+        <v>178</v>
+      </c>
+      <c r="D89" t="s">
+        <v>184</v>
+      </c>
+      <c r="E89" t="s">
+        <v>185</v>
+      </c>
+      <c r="F89" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>176</v>
+      </c>
+      <c r="B90">
+        <v>2014</v>
+      </c>
+      <c r="C90" t="s">
+        <v>179</v>
+      </c>
+      <c r="D90" t="s">
+        <v>187</v>
+      </c>
+      <c r="E90" t="s">
+        <v>188</v>
+      </c>
+      <c r="F90" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>189</v>
+      </c>
+      <c r="B92">
+        <v>2011</v>
+      </c>
+      <c r="C92" t="s">
+        <v>87</v>
+      </c>
+      <c r="D92" t="s">
+        <v>190</v>
+      </c>
+      <c r="E92" t="s">
+        <v>191</v>
+      </c>
+      <c r="F92" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>189</v>
+      </c>
+      <c r="B93">
+        <v>2012</v>
+      </c>
+      <c r="C93" t="s">
+        <v>190</v>
+      </c>
+      <c r="D93" t="s">
+        <v>192</v>
+      </c>
+      <c r="E93" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>189</v>
+      </c>
+      <c r="B94">
+        <v>2013</v>
+      </c>
+      <c r="C94" t="s">
+        <v>193</v>
+      </c>
+      <c r="D94" t="s">
+        <v>190</v>
+      </c>
+      <c r="E94" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>189</v>
+      </c>
+      <c r="B95">
+        <v>2014</v>
+      </c>
+      <c r="C95" t="s">
+        <v>194</v>
+      </c>
+      <c r="D95" t="s">
+        <v>195</v>
+      </c>
+      <c r="E95" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>197</v>
+      </c>
+      <c r="B97">
+        <v>2011</v>
+      </c>
+      <c r="C97" t="s">
+        <v>198</v>
+      </c>
+      <c r="D97" t="s">
+        <v>199</v>
+      </c>
+      <c r="E97" t="s">
+        <v>200</v>
+      </c>
+      <c r="F97" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>197</v>
+      </c>
+      <c r="B98">
+        <v>2012</v>
+      </c>
+      <c r="C98" t="s">
+        <v>203</v>
+      </c>
+      <c r="D98" t="s">
+        <v>199</v>
+      </c>
+      <c r="E98" t="s">
+        <v>80</v>
+      </c>
+      <c r="F98" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>197</v>
+      </c>
+      <c r="B99">
+        <v>2013</v>
+      </c>
+      <c r="C99" t="s">
+        <v>203</v>
+      </c>
+      <c r="D99" t="s">
+        <v>80</v>
+      </c>
+      <c r="E99" t="s">
+        <v>200</v>
+      </c>
+      <c r="F99" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>197</v>
+      </c>
+      <c r="B100">
+        <v>2014</v>
+      </c>
+      <c r="C100" t="s">
+        <v>203</v>
+      </c>
+      <c r="D100" t="s">
+        <v>184</v>
+      </c>
+      <c r="E100" t="s">
+        <v>80</v>
+      </c>
+      <c r="F100" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>205</v>
+      </c>
+      <c r="B102">
+        <v>2011</v>
+      </c>
+      <c r="C102" t="s">
+        <v>207</v>
+      </c>
+      <c r="D102" t="s">
+        <v>208</v>
+      </c>
+      <c r="E102" t="s">
+        <v>209</v>
+      </c>
+      <c r="F102" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>205</v>
+      </c>
+      <c r="B103">
+        <v>2012</v>
+      </c>
+      <c r="C103" t="s">
+        <v>142</v>
+      </c>
+      <c r="D103" t="s">
+        <v>207</v>
+      </c>
+      <c r="E103" t="s">
+        <v>208</v>
+      </c>
+      <c r="F103" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>205</v>
+      </c>
+      <c r="B104">
+        <v>2013</v>
+      </c>
+      <c r="C104" t="s">
+        <v>211</v>
+      </c>
+      <c r="D104" t="s">
+        <v>207</v>
+      </c>
+      <c r="E104" t="s">
+        <v>212</v>
+      </c>
+      <c r="F104" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>205</v>
+      </c>
+      <c r="B105">
+        <v>2014</v>
+      </c>
+      <c r="C105" t="s">
+        <v>211</v>
+      </c>
+      <c r="D105" t="s">
+        <v>207</v>
+      </c>
+      <c r="E105" t="s">
+        <v>212</v>
+      </c>
+      <c r="F105" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>214</v>
+      </c>
+      <c r="B107">
+        <v>2011</v>
+      </c>
+      <c r="C107" t="s">
+        <v>215</v>
+      </c>
+      <c r="D107" t="s">
+        <v>216</v>
+      </c>
+      <c r="E107" t="s">
+        <v>217</v>
+      </c>
+      <c r="F107" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108">
+        <v>2012</v>
+      </c>
+      <c r="C108" t="s">
+        <v>215</v>
+      </c>
+      <c r="D108" t="s">
+        <v>220</v>
+      </c>
+      <c r="E108" t="s">
+        <v>216</v>
+      </c>
+      <c r="F108" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>214</v>
+      </c>
+      <c r="B109">
+        <v>2013</v>
+      </c>
+      <c r="C109" t="s">
+        <v>215</v>
+      </c>
+      <c r="D109" t="s">
+        <v>222</v>
+      </c>
+      <c r="E109" t="s">
+        <v>208</v>
+      </c>
+      <c r="F109" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>214</v>
+      </c>
+      <c r="B110">
+        <v>2014</v>
+      </c>
+      <c r="C110" t="s">
+        <v>224</v>
+      </c>
+      <c r="D110" t="s">
+        <v>208</v>
+      </c>
+      <c r="E110" t="s">
+        <v>225</v>
+      </c>
+      <c r="F110" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>226</v>
+      </c>
+      <c r="B112">
+        <v>2011</v>
+      </c>
+      <c r="C112" t="s">
+        <v>228</v>
+      </c>
+      <c r="D112" t="s">
+        <v>229</v>
+      </c>
+      <c r="E112" t="s">
+        <v>230</v>
+      </c>
+      <c r="F112" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>226</v>
+      </c>
+      <c r="B113">
+        <v>2012</v>
+      </c>
+      <c r="C113" t="s">
+        <v>31</v>
+      </c>
+      <c r="D113" t="s">
+        <v>230</v>
+      </c>
+      <c r="E113" t="s">
+        <v>134</v>
+      </c>
+      <c r="F113" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114">
+        <v>2013</v>
+      </c>
+      <c r="C114" t="s">
+        <v>230</v>
+      </c>
+      <c r="D114" t="s">
+        <v>31</v>
+      </c>
+      <c r="E114" t="s">
+        <v>233</v>
+      </c>
+      <c r="F114" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>226</v>
+      </c>
+      <c r="B115">
+        <v>2014</v>
+      </c>
+      <c r="C115" t="s">
+        <v>230</v>
+      </c>
+      <c r="D115" t="s">
+        <v>233</v>
+      </c>
+      <c r="E115" t="s">
+        <v>31</v>
+      </c>
+      <c r="F115" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>235</v>
+      </c>
+      <c r="B117">
+        <v>2011</v>
+      </c>
+      <c r="C117" t="s">
+        <v>237</v>
+      </c>
+      <c r="D117" t="s">
+        <v>238</v>
+      </c>
+      <c r="E117" t="s">
+        <v>239</v>
+      </c>
+      <c r="F117" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>235</v>
+      </c>
+      <c r="B118">
+        <v>2012</v>
+      </c>
+      <c r="C118" t="s">
+        <v>240</v>
+      </c>
+      <c r="D118" t="s">
+        <v>237</v>
+      </c>
+      <c r="E118" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>235</v>
+      </c>
+      <c r="B119">
+        <v>2013</v>
+      </c>
+      <c r="C119" t="s">
+        <v>237</v>
+      </c>
+      <c r="D119" t="s">
+        <v>242</v>
+      </c>
+      <c r="E119" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>235</v>
+      </c>
+      <c r="B120">
+        <v>2014</v>
+      </c>
+      <c r="C120" t="s">
+        <v>237</v>
+      </c>
+      <c r="D120" t="s">
+        <v>242</v>
+      </c>
+      <c r="E120" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>244</v>
+      </c>
+      <c r="B122">
+        <v>2011</v>
+      </c>
+      <c r="C122" t="s">
+        <v>77</v>
+      </c>
+      <c r="D122" t="s">
+        <v>246</v>
+      </c>
+      <c r="E122" t="s">
+        <v>247</v>
+      </c>
+      <c r="F122" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123">
+        <v>2012</v>
+      </c>
+      <c r="C123" t="s">
+        <v>246</v>
+      </c>
+      <c r="D123" t="s">
+        <v>158</v>
+      </c>
+      <c r="E123" t="s">
+        <v>248</v>
+      </c>
+      <c r="F123" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>244</v>
+      </c>
+      <c r="B124">
+        <v>2013</v>
+      </c>
+      <c r="C124" t="s">
+        <v>158</v>
+      </c>
+      <c r="D124" t="s">
+        <v>248</v>
+      </c>
+      <c r="E124" t="s">
+        <v>12</v>
+      </c>
+      <c r="F124" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>244</v>
+      </c>
+      <c r="B125">
+        <v>2014</v>
+      </c>
+      <c r="C125" t="s">
+        <v>250</v>
+      </c>
+      <c r="D125" t="s">
+        <v>248</v>
+      </c>
+      <c r="E125" t="s">
+        <v>247</v>
+      </c>
+      <c r="F125" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>251</v>
+      </c>
+      <c r="B127">
+        <v>2011</v>
+      </c>
+      <c r="C127" t="s">
+        <v>253</v>
+      </c>
+      <c r="D127" t="s">
+        <v>254</v>
+      </c>
+      <c r="E127" t="s">
+        <v>255</v>
+      </c>
+      <c r="F127" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>251</v>
+      </c>
+      <c r="B128">
+        <v>2012</v>
+      </c>
+      <c r="C128" t="s">
+        <v>253</v>
+      </c>
+      <c r="D128" t="s">
+        <v>255</v>
+      </c>
+      <c r="E128" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>251</v>
+      </c>
+      <c r="B129">
+        <v>2013</v>
+      </c>
+      <c r="C129" t="s">
+        <v>256</v>
+      </c>
+      <c r="D129" t="s">
+        <v>257</v>
+      </c>
+      <c r="E129" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>251</v>
+      </c>
+      <c r="B130">
+        <v>2014</v>
+      </c>
+      <c r="C130" t="s">
+        <v>254</v>
+      </c>
+      <c r="D130" t="s">
+        <v>255</v>
+      </c>
+      <c r="E130" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>259</v>
+      </c>
+      <c r="B132">
+        <v>2011</v>
+      </c>
+      <c r="C132" t="s">
+        <v>261</v>
+      </c>
+      <c r="D132" t="s">
+        <v>262</v>
+      </c>
+      <c r="E132" t="s">
+        <v>265</v>
+      </c>
+      <c r="F132" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>259</v>
+      </c>
+      <c r="B133">
+        <v>2012</v>
+      </c>
+      <c r="C133" t="s">
+        <v>264</v>
+      </c>
+      <c r="D133" t="s">
+        <v>265</v>
+      </c>
+      <c r="E133" t="s">
+        <v>159</v>
+      </c>
+      <c r="F133" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>259</v>
+      </c>
+      <c r="B134">
+        <v>2013</v>
+      </c>
+      <c r="C134" t="s">
+        <v>159</v>
+      </c>
+      <c r="D134" t="s">
+        <v>266</v>
+      </c>
+      <c r="E134" t="s">
+        <v>267</v>
+      </c>
+      <c r="F134" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>259</v>
+      </c>
+      <c r="B135">
+        <v>2014</v>
+      </c>
+      <c r="C135" t="s">
+        <v>270</v>
+      </c>
+      <c r="D135" t="s">
+        <v>159</v>
+      </c>
+      <c r="E135" t="s">
+        <v>264</v>
+      </c>
+      <c r="F135" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>271</v>
+      </c>
+      <c r="B137">
+        <v>2011</v>
+      </c>
+      <c r="C137" t="s">
+        <v>272</v>
+      </c>
+      <c r="D137" t="s">
+        <v>188</v>
+      </c>
+      <c r="E137" t="s">
+        <v>273</v>
+      </c>
+      <c r="F137" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>271</v>
+      </c>
+      <c r="B138">
+        <v>2012</v>
+      </c>
+      <c r="C138" t="s">
+        <v>273</v>
+      </c>
+      <c r="D138" t="s">
+        <v>272</v>
+      </c>
+      <c r="E138" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>271</v>
+      </c>
+      <c r="B139">
+        <v>2013</v>
+      </c>
+      <c r="C139" t="s">
+        <v>272</v>
+      </c>
+      <c r="D139" t="s">
+        <v>273</v>
+      </c>
+      <c r="E139" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>271</v>
+      </c>
+      <c r="B140">
+        <v>2014</v>
+      </c>
+      <c r="C140" t="s">
+        <v>272</v>
+      </c>
+      <c r="D140" t="s">
+        <v>277</v>
+      </c>
+      <c r="E140" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>278</v>
+      </c>
+      <c r="B142">
+        <v>2011</v>
+      </c>
+      <c r="C142" t="s">
+        <v>280</v>
+      </c>
+      <c r="D142" t="s">
+        <v>281</v>
+      </c>
+      <c r="E142" t="s">
+        <v>282</v>
+      </c>
+      <c r="F142" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>278</v>
+      </c>
+      <c r="B143">
+        <v>2012</v>
+      </c>
+      <c r="C143" t="s">
+        <v>284</v>
+      </c>
+      <c r="D143" t="s">
+        <v>280</v>
+      </c>
+      <c r="E143" t="s">
+        <v>281</v>
+      </c>
+      <c r="F143" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>278</v>
+      </c>
+      <c r="B144">
+        <v>2013</v>
+      </c>
+      <c r="C144" t="s">
+        <v>281</v>
+      </c>
+      <c r="D144" t="s">
+        <v>47</v>
+      </c>
+      <c r="E144" t="s">
+        <v>286</v>
+      </c>
+      <c r="F144" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>278</v>
+      </c>
+      <c r="B145">
+        <v>2014</v>
+      </c>
+      <c r="C145" t="s">
+        <v>286</v>
+      </c>
+      <c r="D145" t="s">
+        <v>288</v>
+      </c>
+      <c r="E145" t="s">
+        <v>289</v>
+      </c>
+      <c r="F145" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>290</v>
+      </c>
+      <c r="B147">
+        <v>2011</v>
+      </c>
+      <c r="C147" t="s">
+        <v>257</v>
+      </c>
+      <c r="D147" t="s">
+        <v>293</v>
+      </c>
+      <c r="E147" t="s">
+        <v>161</v>
+      </c>
+      <c r="F147" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>290</v>
+      </c>
+      <c r="B148">
+        <v>2012</v>
+      </c>
+      <c r="C148" t="s">
+        <v>294</v>
+      </c>
+      <c r="D148" t="s">
+        <v>257</v>
+      </c>
+      <c r="E148" t="s">
+        <v>295</v>
+      </c>
+      <c r="F148" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>290</v>
+      </c>
+      <c r="B149">
+        <v>2013</v>
+      </c>
+      <c r="C149" t="s">
+        <v>297</v>
+      </c>
+      <c r="D149" t="s">
+        <v>298</v>
+      </c>
+      <c r="E149" t="s">
+        <v>299</v>
+      </c>
+      <c r="F149" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>290</v>
+      </c>
+      <c r="B150">
+        <v>2014</v>
+      </c>
+      <c r="C150" t="s">
+        <v>301</v>
+      </c>
+      <c r="D150" t="s">
+        <v>295</v>
+      </c>
+      <c r="E150" t="s">
+        <v>302</v>
+      </c>
+      <c r="F150" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>303</v>
+      </c>
+      <c r="B152">
+        <v>2011</v>
+      </c>
+      <c r="C152" t="s">
+        <v>305</v>
+      </c>
+      <c r="D152" t="s">
+        <v>306</v>
+      </c>
+      <c r="E152" t="s">
+        <v>243</v>
+      </c>
+      <c r="F152" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>303</v>
+      </c>
+      <c r="B153">
+        <v>2012</v>
+      </c>
+      <c r="C153" t="s">
+        <v>305</v>
+      </c>
+      <c r="D153" t="s">
+        <v>308</v>
+      </c>
+      <c r="E153" t="s">
+        <v>243</v>
+      </c>
+      <c r="F153" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>303</v>
+      </c>
+      <c r="B154">
+        <v>2013</v>
+      </c>
+      <c r="C154" t="s">
+        <v>305</v>
+      </c>
+      <c r="D154" t="s">
+        <v>243</v>
+      </c>
+      <c r="E154" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>303</v>
+      </c>
+      <c r="B155">
+        <v>2014</v>
+      </c>
+      <c r="C155" t="s">
+        <v>305</v>
+      </c>
+      <c r="D155" t="s">
+        <v>306</v>
+      </c>
+      <c r="E155" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>310</v>
+      </c>
+      <c r="B157">
+        <v>2011</v>
+      </c>
+      <c r="C157" t="s">
+        <v>313</v>
+      </c>
+      <c r="D157" t="s">
+        <v>312</v>
+      </c>
+      <c r="E157" t="s">
+        <v>314</v>
+      </c>
+      <c r="F157" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>310</v>
+      </c>
+      <c r="B158">
+        <v>2012</v>
+      </c>
+      <c r="C158" t="s">
+        <v>313</v>
+      </c>
+      <c r="D158" t="s">
+        <v>314</v>
+      </c>
+      <c r="E158" t="s">
+        <v>312</v>
+      </c>
+      <c r="F158" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>310</v>
+      </c>
+      <c r="B159">
+        <v>2013</v>
+      </c>
+      <c r="C159" t="s">
+        <v>312</v>
+      </c>
+      <c r="D159" t="s">
+        <v>313</v>
+      </c>
+      <c r="E159" t="s">
+        <v>316</v>
+      </c>
+      <c r="F159" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>310</v>
+      </c>
+      <c r="B160">
+        <v>2014</v>
+      </c>
+      <c r="C160" t="s">
+        <v>313</v>
+      </c>
+      <c r="D160" t="s">
+        <v>316</v>
+      </c>
+      <c r="E160" t="s">
+        <v>314</v>
+      </c>
+      <c r="F160" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>